<commit_message>
Initial commit with frontend and backend
</commit_message>
<xml_diff>
--- a/backend/data.xlsx
+++ b/backend/data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H119"/>
+  <dimension ref="A1:H134"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -3034,9 +3034,354 @@
         <v>2025-02-07T18:30:00.000Z</v>
       </c>
     </row>
+    <row r="120">
+      <c r="A120" t="str">
+        <v>Prajwal Gajanan Wani</v>
+      </c>
+      <c r="B120" t="str">
+        <v>9096609945</v>
+      </c>
+      <c r="C120" t="str">
+        <v>Kothrud</v>
+      </c>
+      <c r="D120" t="str">
+        <v>Sai Nagar</v>
+      </c>
+      <c r="E120" t="str">
+        <v>30/1/2025, 6:05:08 pm</v>
+      </c>
+      <c r="F120" t="str">
+        <v>pending</v>
+      </c>
+      <c r="G120" t="str">
+        <v>2025-02-21T18:30:00.000Z</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="str">
+        <v>Prajwal Gajanan Wani</v>
+      </c>
+      <c r="B121" t="str">
+        <v>9096609945</v>
+      </c>
+      <c r="C121" t="str">
+        <v>Kothrud</v>
+      </c>
+      <c r="D121" t="str">
+        <v>Sai Nagar</v>
+      </c>
+      <c r="E121" t="str">
+        <v>30/1/2025, 6:29:31 pm</v>
+      </c>
+      <c r="F121" t="str">
+        <v>pending</v>
+      </c>
+      <c r="G121" t="str">
+        <v>2025-03-07T18:30:00.000Z</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="str">
+        <v>Prajwal Gajanan Wani</v>
+      </c>
+      <c r="B122" t="str">
+        <v>9096609945</v>
+      </c>
+      <c r="C122" t="str">
+        <v>Kothrud</v>
+      </c>
+      <c r="D122" t="str">
+        <v>Sai Nagar</v>
+      </c>
+      <c r="E122" t="str">
+        <v>30/1/2025, 6:48:50 pm</v>
+      </c>
+      <c r="F122" t="str">
+        <v>pending</v>
+      </c>
+      <c r="G122" t="str">
+        <v>2025-02-21T18:30:00.000Z</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="str">
+        <v>Prajwal Gajanan Wani</v>
+      </c>
+      <c r="B123" t="str">
+        <v>9096609945</v>
+      </c>
+      <c r="C123" t="str">
+        <v>Kothrud</v>
+      </c>
+      <c r="D123" t="str">
+        <v>Sai Nagar</v>
+      </c>
+      <c r="E123" t="str">
+        <v>30/1/2025, 6:53:19 pm</v>
+      </c>
+      <c r="F123" t="str">
+        <v>pending</v>
+      </c>
+      <c r="G123" t="str">
+        <v>2025-02-21T18:30:00.000Z</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="str">
+        <v>Prajwal Gajanan Wani</v>
+      </c>
+      <c r="B124" t="str">
+        <v>9096609945</v>
+      </c>
+      <c r="C124" t="str">
+        <v>Kothrud</v>
+      </c>
+      <c r="D124" t="str">
+        <v>Sai Nagar</v>
+      </c>
+      <c r="E124" t="str">
+        <v>30/1/2025, 6:56:10 pm</v>
+      </c>
+      <c r="F124" t="str">
+        <v>pending</v>
+      </c>
+      <c r="G124" t="str">
+        <v>2025-02-07T18:30:00.000Z</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="str">
+        <v>Prajwal Gajanan Wani</v>
+      </c>
+      <c r="B125" t="str">
+        <v>9096609945</v>
+      </c>
+      <c r="C125" t="str">
+        <v>Kothrud</v>
+      </c>
+      <c r="D125" t="str">
+        <v>Sai Nagar</v>
+      </c>
+      <c r="E125" t="str">
+        <v>30/1/2025, 11:26:52 pm</v>
+      </c>
+      <c r="F125" t="str">
+        <v>pending</v>
+      </c>
+      <c r="G125" t="str">
+        <v>2025-02-21T18:30:00.000Z</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="str">
+        <v>Prajwal Gajanan Wani</v>
+      </c>
+      <c r="B126" t="str">
+        <v>9096609945</v>
+      </c>
+      <c r="C126" t="str">
+        <v>Kothrud</v>
+      </c>
+      <c r="D126" t="str">
+        <v>Sai Nagar</v>
+      </c>
+      <c r="E126" t="str">
+        <v>31/1/2025, 3:37:54 pm</v>
+      </c>
+      <c r="F126" t="str">
+        <v>pending</v>
+      </c>
+      <c r="G126" t="str">
+        <v>2025-02-14T18:30:00.000Z</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="str">
+        <v>Prajwal Gajanan Wani</v>
+      </c>
+      <c r="B127" t="str">
+        <v>9096609945</v>
+      </c>
+      <c r="C127" t="str">
+        <v>Kothrud</v>
+      </c>
+      <c r="D127" t="str">
+        <v>Sai Nagar</v>
+      </c>
+      <c r="E127" t="str">
+        <v>3/2/2025, 10:45:45 am</v>
+      </c>
+      <c r="F127" t="str">
+        <v>pending</v>
+      </c>
+      <c r="G127" t="str">
+        <v>2025-02-21T18:30:00.000Z</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="str">
+        <v>Prajwal Gajanan Wani</v>
+      </c>
+      <c r="B128" t="str">
+        <v>9096609945</v>
+      </c>
+      <c r="C128" t="str">
+        <v>Kothrud</v>
+      </c>
+      <c r="D128" t="str">
+        <v>Sai Nagar</v>
+      </c>
+      <c r="E128" t="str">
+        <v>3/2/2025, 10:56:13 am</v>
+      </c>
+      <c r="F128" t="str">
+        <v>pending</v>
+      </c>
+      <c r="G128" t="str">
+        <v>2025-02-21T18:30:00.000Z</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="str">
+        <v>Prajwal Gajanan Wani</v>
+      </c>
+      <c r="B129" t="str">
+        <v>9096609945</v>
+      </c>
+      <c r="C129" t="str">
+        <v>Kothrud</v>
+      </c>
+      <c r="D129" t="str">
+        <v>Sai Nagar</v>
+      </c>
+      <c r="E129" t="str">
+        <v>3/2/2025, 10:58:47 am</v>
+      </c>
+      <c r="F129" t="str">
+        <v>pending</v>
+      </c>
+      <c r="G129" t="str">
+        <v>2025-02-14T18:30:00.000Z</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="str">
+        <v>Prajwal Gajanan Wani</v>
+      </c>
+      <c r="B130" t="str">
+        <v>9096609945</v>
+      </c>
+      <c r="C130" t="str">
+        <v>Kothrud</v>
+      </c>
+      <c r="D130" t="str">
+        <v>Sai Nagar</v>
+      </c>
+      <c r="E130" t="str">
+        <v>3/2/2025, 11:48:48 am</v>
+      </c>
+      <c r="F130" t="str">
+        <v>pending</v>
+      </c>
+      <c r="G130" t="str">
+        <v>2025-04-11T18:30:00.000Z</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="str">
+        <v>Prajwal Gajanan Wani</v>
+      </c>
+      <c r="B131" t="str">
+        <v>9096609945</v>
+      </c>
+      <c r="C131" t="str">
+        <v>Kothrud</v>
+      </c>
+      <c r="D131" t="str">
+        <v>Sai Nagar</v>
+      </c>
+      <c r="E131" t="str">
+        <v>3/2/2025, 8:07:35 pm</v>
+      </c>
+      <c r="F131" t="str">
+        <v>pending</v>
+      </c>
+      <c r="G131" t="str">
+        <v>2025-02-21T18:30:00.000Z</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="str">
+        <v>Prajwal Gajanan Wani</v>
+      </c>
+      <c r="B132" t="str">
+        <v>9096609945</v>
+      </c>
+      <c r="C132" t="str">
+        <v>Kothrud</v>
+      </c>
+      <c r="D132" t="str">
+        <v>Sai Nagar</v>
+      </c>
+      <c r="E132" t="str">
+        <v>3/2/2025, 8:16:18 pm</v>
+      </c>
+      <c r="F132" t="str">
+        <v>pending</v>
+      </c>
+      <c r="G132" t="str">
+        <v>2025-02-21T18:30:00.000Z</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="str">
+        <v>Prajwal Gajanan Wani</v>
+      </c>
+      <c r="B133" t="str">
+        <v>9096609945</v>
+      </c>
+      <c r="C133" t="str">
+        <v>Kothrud</v>
+      </c>
+      <c r="D133" t="str">
+        <v>Sai Nagar</v>
+      </c>
+      <c r="E133" t="str">
+        <v>4/2/2025, 11:40:46 am</v>
+      </c>
+      <c r="F133" t="str">
+        <v>pending</v>
+      </c>
+      <c r="G133" t="str">
+        <v>2025-03-28T18:30:00.000Z</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="str">
+        <v>Prajwal Gajanan Wani</v>
+      </c>
+      <c r="B134" t="str">
+        <v>9096609945</v>
+      </c>
+      <c r="C134" t="str">
+        <v>Kothrud</v>
+      </c>
+      <c r="D134" t="str">
+        <v>Sai Nagar</v>
+      </c>
+      <c r="E134" t="str">
+        <v>4/2/2025, 1:29:52 pm</v>
+      </c>
+      <c r="F134" t="str">
+        <v>pending</v>
+      </c>
+      <c r="G134" t="str">
+        <v>2025-02-22T18:30:00.000Z</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H119"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H134"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>